<commit_message>
Update Mayoral Race folder
</commit_message>
<xml_diff>
--- a/MayoralRaceResult/Data/voterTurnout.xlsx
+++ b/MayoralRaceResult/Data/voterTurnout.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hata/Documents/thescopeboston.github.io/MayoralRaceResult/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E001CD0-B25A-794B-B47E-F8040C39560D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FE3193F-080D-F740-9B68-E070E8BD7589}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{79F5E2FA-45EF-5147-B6C8-3ED9BB1C561A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16020" xr2:uid="{79F5E2FA-45EF-5147-B6C8-3ED9BB1C561A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2952,8 +2952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9380636-B0A5-6945-B2B3-0A9ACD81E8E7}">
   <dimension ref="A1:E257"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="G69" sqref="G69"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2992,7 +2992,7 @@
         <v>1203</v>
       </c>
       <c r="D2" s="6">
-        <f>B2/C2*100</f>
+        <f t="shared" ref="D2:D65" si="0">B2/C2*100</f>
         <v>63.175394846217792</v>
       </c>
       <c r="E2" s="8">
@@ -3010,7 +3010,7 @@
         <v>1203</v>
       </c>
       <c r="D3" s="6">
-        <f>B3/C3*100</f>
+        <f t="shared" si="0"/>
         <v>63.175394846217792</v>
       </c>
       <c r="E3" s="8">
@@ -3028,7 +3028,7 @@
         <v>989</v>
       </c>
       <c r="D4" s="6">
-        <f>B4/C4*100</f>
+        <f t="shared" si="0"/>
         <v>56.31951466127402</v>
       </c>
       <c r="E4" s="8">
@@ -3046,7 +3046,7 @@
         <v>1113</v>
       </c>
       <c r="D5" s="6">
-        <f>B5/C5*100</f>
+        <f t="shared" si="0"/>
         <v>52.650494159928115</v>
       </c>
       <c r="E5" s="8">
@@ -3064,7 +3064,7 @@
         <v>879</v>
       </c>
       <c r="D6" s="6">
-        <f>B6/C6*100</f>
+        <f t="shared" si="0"/>
         <v>51.649601820250282</v>
       </c>
       <c r="E6" s="8">
@@ -3082,7 +3082,7 @@
         <v>1714</v>
       </c>
       <c r="D7" s="6">
-        <f>B7/C7*100</f>
+        <f t="shared" si="0"/>
         <v>50.875145857642948</v>
       </c>
       <c r="E7" s="8">
@@ -3100,7 +3100,7 @@
         <v>1029</v>
       </c>
       <c r="D8" s="6">
-        <f>B8/C8*100</f>
+        <f t="shared" si="0"/>
         <v>49.854227405247812</v>
       </c>
       <c r="E8" s="8">
@@ -3118,7 +3118,7 @@
         <v>1085</v>
       </c>
       <c r="D9" s="6">
-        <f>B9/C9*100</f>
+        <f t="shared" si="0"/>
         <v>49.585253456221196</v>
       </c>
       <c r="E9" s="8">
@@ -3136,7 +3136,7 @@
         <v>1589</v>
       </c>
       <c r="D10" s="6">
-        <f>B10/C10*100</f>
+        <f t="shared" si="0"/>
         <v>48.206419131529266</v>
       </c>
       <c r="E10" s="8">
@@ -3154,7 +3154,7 @@
         <v>1311</v>
       </c>
       <c r="D11" s="6">
-        <f>B11/C11*100</f>
+        <f t="shared" si="0"/>
         <v>46.834477498093058</v>
       </c>
       <c r="E11" s="8">
@@ -3172,7 +3172,7 @@
         <v>1567</v>
       </c>
       <c r="D12" s="6">
-        <f>B12/C12*100</f>
+        <f t="shared" si="0"/>
         <v>46.075303126994257</v>
       </c>
       <c r="E12" s="8">
@@ -3190,7 +3190,7 @@
         <v>1567</v>
       </c>
       <c r="D13" s="6">
-        <f>B13/C13*100</f>
+        <f t="shared" si="0"/>
         <v>46.075303126994257</v>
       </c>
       <c r="E13" s="8">
@@ -3208,7 +3208,7 @@
         <v>1102</v>
       </c>
       <c r="D14" s="6">
-        <f>B14/C14*100</f>
+        <f t="shared" si="0"/>
         <v>45.825771324863886</v>
       </c>
       <c r="E14" s="8">
@@ -3226,7 +3226,7 @@
         <v>1079</v>
       </c>
       <c r="D15" s="6">
-        <f>B15/C15*100</f>
+        <f t="shared" si="0"/>
         <v>45.597775718257644</v>
       </c>
       <c r="E15" s="8">
@@ -3244,7 +3244,7 @@
         <v>929</v>
       </c>
       <c r="D16" s="6">
-        <f>B16/C16*100</f>
+        <f t="shared" si="0"/>
         <v>45.317545748116252</v>
       </c>
       <c r="E16" s="8">
@@ -3262,7 +3262,7 @@
         <v>1229</v>
       </c>
       <c r="D17" s="6">
-        <f>B17/C17*100</f>
+        <f t="shared" si="0"/>
         <v>44.507729861676161</v>
       </c>
       <c r="E17" s="8">
@@ -3280,7 +3280,7 @@
         <v>2099</v>
       </c>
       <c r="D18" s="6">
-        <f>B18/C18*100</f>
+        <f t="shared" si="0"/>
         <v>44.449737970462124</v>
       </c>
       <c r="E18" s="8">
@@ -3298,7 +3298,7 @@
         <v>1778</v>
       </c>
       <c r="D19" s="6">
-        <f>B19/C19*100</f>
+        <f t="shared" si="0"/>
         <v>42.463442069741284</v>
       </c>
       <c r="E19" s="8">
@@ -3316,7 +3316,7 @@
         <v>899</v>
       </c>
       <c r="D20" s="6">
-        <f>B20/C20*100</f>
+        <f t="shared" si="0"/>
         <v>42.157953281423808</v>
       </c>
       <c r="E20" s="8">
@@ -3334,7 +3334,7 @@
         <v>1328</v>
       </c>
       <c r="D21" s="6">
-        <f>B21/C21*100</f>
+        <f t="shared" si="0"/>
         <v>41.415662650602407</v>
       </c>
       <c r="E21" s="8">
@@ -3352,7 +3352,7 @@
         <v>1328</v>
       </c>
       <c r="D22" s="6">
-        <f>B22/C22*100</f>
+        <f t="shared" si="0"/>
         <v>41.415662650602407</v>
       </c>
       <c r="E22" s="8">
@@ -3370,7 +3370,7 @@
         <v>2099</v>
       </c>
       <c r="D23" s="6">
-        <f>B23/C23*100</f>
+        <f t="shared" si="0"/>
         <v>41.210100047641731</v>
       </c>
       <c r="E23" s="8">
@@ -3388,7 +3388,7 @@
         <v>1409</v>
       </c>
       <c r="D24" s="6">
-        <f>B24/C24*100</f>
+        <f t="shared" si="0"/>
         <v>41.163946061036192</v>
       </c>
       <c r="E24" s="8">
@@ -3406,7 +3406,7 @@
         <v>1900</v>
       </c>
       <c r="D25" s="6">
-        <f>B25/C25*100</f>
+        <f t="shared" si="0"/>
         <v>41.10526315789474</v>
       </c>
       <c r="E25" s="8">
@@ -3424,7 +3424,7 @@
         <v>1512</v>
       </c>
       <c r="D26" s="6">
-        <f>B26/C26*100</f>
+        <f t="shared" si="0"/>
         <v>41.005291005291006</v>
       </c>
       <c r="E26" s="8">
@@ -3442,7 +3442,7 @@
         <v>1512</v>
       </c>
       <c r="D27" s="6">
-        <f>B27/C27*100</f>
+        <f t="shared" si="0"/>
         <v>41.005291005291006</v>
       </c>
       <c r="E27" s="8">
@@ -3460,7 +3460,7 @@
         <v>1217</v>
       </c>
       <c r="D28" s="6">
-        <f>B28/C28*100</f>
+        <f t="shared" si="0"/>
         <v>40.591618734593261</v>
       </c>
       <c r="E28" s="8">
@@ -3478,7 +3478,7 @@
         <v>1082</v>
       </c>
       <c r="D29" s="6">
-        <f>B29/C29*100</f>
+        <f t="shared" si="0"/>
         <v>40.480591497227358</v>
       </c>
       <c r="E29" s="8">
@@ -3496,7 +3496,7 @@
         <v>1605</v>
       </c>
       <c r="D30" s="6">
-        <f>B30/C30*100</f>
+        <f t="shared" si="0"/>
         <v>39.439252336448597</v>
       </c>
       <c r="E30" s="8">
@@ -3514,7 +3514,7 @@
         <v>1520</v>
       </c>
       <c r="D31" s="6">
-        <f>B31/C31*100</f>
+        <f t="shared" si="0"/>
         <v>39.407894736842103</v>
       </c>
       <c r="E31" s="8">
@@ -3532,7 +3532,7 @@
         <v>1520</v>
       </c>
       <c r="D32" s="6">
-        <f>B32/C32*100</f>
+        <f t="shared" si="0"/>
         <v>39.407894736842103</v>
       </c>
       <c r="E32" s="8">
@@ -3550,7 +3550,7 @@
         <v>1867</v>
       </c>
       <c r="D33" s="6">
-        <f>B33/C33*100</f>
+        <f t="shared" si="0"/>
         <v>39.260846277450455</v>
       </c>
       <c r="E33" s="8">
@@ -3568,7 +3568,7 @@
         <v>1694</v>
       </c>
       <c r="D34" s="6">
-        <f>B34/C34*100</f>
+        <f t="shared" si="0"/>
         <v>38.902007083825261</v>
       </c>
       <c r="E34" s="8">
@@ -3586,7 +3586,7 @@
         <v>1457</v>
       </c>
       <c r="D35" s="6">
-        <f>B35/C35*100</f>
+        <f t="shared" si="0"/>
         <v>38.846945778997942</v>
       </c>
       <c r="E35" s="8">
@@ -3604,7 +3604,7 @@
         <v>2026</v>
       </c>
       <c r="D36" s="6">
-        <f>B36/C36*100</f>
+        <f t="shared" si="0"/>
         <v>38.6969397828233</v>
       </c>
       <c r="E36" s="8">
@@ -3622,7 +3622,7 @@
         <v>1846</v>
       </c>
       <c r="D37" s="6">
-        <f>B37/C37*100</f>
+        <f t="shared" si="0"/>
         <v>38.678223185265438</v>
       </c>
       <c r="E37" s="8">
@@ -3640,7 +3640,7 @@
         <v>1273</v>
       </c>
       <c r="D38" s="6">
-        <f>B38/C38*100</f>
+        <f t="shared" si="0"/>
         <v>38.491751767478398</v>
       </c>
       <c r="E38" s="8">
@@ -3658,7 +3658,7 @@
         <v>1916</v>
       </c>
       <c r="D39" s="6">
-        <f>B39/C39*100</f>
+        <f t="shared" si="0"/>
         <v>37.578288100208766</v>
       </c>
       <c r="E39" s="8">
@@ -3676,7 +3676,7 @@
         <v>1792</v>
       </c>
       <c r="D40" s="6">
-        <f>B40/C40*100</f>
+        <f t="shared" si="0"/>
         <v>37.555803571428569</v>
       </c>
       <c r="E40" s="8">
@@ -3694,7 +3694,7 @@
         <v>1949</v>
       </c>
       <c r="D41" s="6">
-        <f>B41/C41*100</f>
+        <f t="shared" si="0"/>
         <v>34.376603386351974</v>
       </c>
       <c r="E41" s="8">
@@ -3712,7 +3712,7 @@
         <v>1313</v>
       </c>
       <c r="D42" s="6">
-        <f>B42/C42*100</f>
+        <f t="shared" si="0"/>
         <v>34.196496572734198</v>
       </c>
       <c r="E42" s="8">
@@ -3730,7 +3730,7 @@
         <v>1764</v>
       </c>
       <c r="D43" s="6">
-        <f>B43/C43*100</f>
+        <f t="shared" si="0"/>
         <v>33.616780045351476</v>
       </c>
       <c r="E43" s="8">
@@ -3748,7 +3748,7 @@
         <v>1466</v>
       </c>
       <c r="D44" s="6">
-        <f>B44/C44*100</f>
+        <f t="shared" si="0"/>
         <v>33.356070941336974</v>
       </c>
       <c r="E44" s="8">
@@ -3766,7 +3766,7 @@
         <v>1522</v>
       </c>
       <c r="D45" s="6">
-        <f>B45/C45*100</f>
+        <f t="shared" si="0"/>
         <v>32.851511169513799</v>
       </c>
       <c r="E45" s="8">
@@ -3784,7 +3784,7 @@
         <v>1522</v>
       </c>
       <c r="D46" s="6">
-        <f>B46/C46*100</f>
+        <f t="shared" si="0"/>
         <v>32.851511169513799</v>
       </c>
       <c r="E46" s="8">
@@ -3802,7 +3802,7 @@
         <v>2041</v>
       </c>
       <c r="D47" s="6">
-        <f>B47/C47*100</f>
+        <f t="shared" si="0"/>
         <v>32.582067613914752</v>
       </c>
       <c r="E47" s="8">
@@ -3820,7 +3820,7 @@
         <v>2146</v>
       </c>
       <c r="D48" s="6">
-        <f>B48/C48*100</f>
+        <f t="shared" si="0"/>
         <v>32.339235787511647</v>
       </c>
       <c r="E48" s="8" t="s">
@@ -3838,7 +3838,7 @@
         <v>2309</v>
       </c>
       <c r="D49" s="6">
-        <f>B49/C49*100</f>
+        <f t="shared" si="0"/>
         <v>31.702035513209182</v>
       </c>
       <c r="E49" s="8">
@@ -3856,7 +3856,7 @@
         <v>1654</v>
       </c>
       <c r="D50" s="6">
-        <f>B50/C50*100</f>
+        <f t="shared" si="0"/>
         <v>31.680773881499398</v>
       </c>
       <c r="E50" s="8" t="s">
@@ -3874,7 +3874,7 @@
         <v>1406</v>
       </c>
       <c r="D51" s="6">
-        <f>B51/C51*100</f>
+        <f t="shared" si="0"/>
         <v>31.0099573257468</v>
       </c>
       <c r="E51" s="8" t="s">
@@ -3892,7 +3892,7 @@
         <v>1877</v>
       </c>
       <c r="D52" s="6">
-        <f>B52/C52*100</f>
+        <f t="shared" si="0"/>
         <v>30.367607884922748</v>
       </c>
       <c r="E52" s="8">
@@ -3910,7 +3910,7 @@
         <v>689</v>
       </c>
       <c r="D53" s="6">
-        <f>B53/C53*100</f>
+        <f t="shared" si="0"/>
         <v>30.188679245283019</v>
       </c>
       <c r="E53" s="8" t="s">
@@ -3928,7 +3928,7 @@
         <v>1754</v>
       </c>
       <c r="D54" s="6">
-        <f>B54/C54*100</f>
+        <f t="shared" si="0"/>
         <v>29.988597491448122</v>
       </c>
       <c r="E54" s="8" t="s">
@@ -3946,7 +3946,7 @@
         <v>2106</v>
       </c>
       <c r="D55" s="6">
-        <f>B55/C55*100</f>
+        <f t="shared" si="0"/>
         <v>29.629629629629626</v>
       </c>
       <c r="E55" s="8">
@@ -3964,7 +3964,7 @@
         <v>2106</v>
       </c>
       <c r="D56" s="6">
-        <f>B56/C56*100</f>
+        <f t="shared" si="0"/>
         <v>29.629629629629626</v>
       </c>
       <c r="E56" s="8">
@@ -3982,7 +3982,7 @@
         <v>1972</v>
       </c>
       <c r="D57" s="6">
-        <f>B57/C57*100</f>
+        <f t="shared" si="0"/>
         <v>29.411764705882355</v>
       </c>
       <c r="E57" s="8" t="s">
@@ -4000,7 +4000,7 @@
         <v>2253</v>
       </c>
       <c r="D58" s="6">
-        <f>B58/C58*100</f>
+        <f t="shared" si="0"/>
         <v>28.806036395916557</v>
       </c>
       <c r="E58" s="8">
@@ -4018,7 +4018,7 @@
         <v>1543</v>
       </c>
       <c r="D59" s="6">
-        <f>B59/C59*100</f>
+        <f t="shared" si="0"/>
         <v>28.775113415424496</v>
       </c>
       <c r="E59" s="8" t="s">
@@ -4036,7 +4036,7 @@
         <v>1025</v>
       </c>
       <c r="D60" s="6">
-        <f>B60/C60*100</f>
+        <f t="shared" si="0"/>
         <v>28.68292682926829</v>
       </c>
       <c r="E60" s="8">
@@ -4054,7 +4054,7 @@
         <v>1025</v>
       </c>
       <c r="D61" s="6">
-        <f>B61/C61*100</f>
+        <f t="shared" si="0"/>
         <v>28.68292682926829</v>
       </c>
       <c r="E61" s="8">
@@ -4072,7 +4072,7 @@
         <v>2350</v>
       </c>
       <c r="D62" s="6">
-        <f>B62/C62*100</f>
+        <f t="shared" si="0"/>
         <v>28.553191489361701</v>
       </c>
       <c r="E62" s="8" t="s">
@@ -4090,7 +4090,7 @@
         <v>754</v>
       </c>
       <c r="D63" s="6">
-        <f>B63/C63*100</f>
+        <f t="shared" si="0"/>
         <v>28.514588859416445</v>
       </c>
       <c r="E63" s="8">
@@ -4108,7 +4108,7 @@
         <v>1705</v>
       </c>
       <c r="D64" s="6">
-        <f>B64/C64*100</f>
+        <f t="shared" si="0"/>
         <v>28.504398826979472</v>
       </c>
       <c r="E64" s="8" t="s">
@@ -4126,7 +4126,7 @@
         <v>2133</v>
       </c>
       <c r="D65" s="6">
-        <f>B65/C65*100</f>
+        <f t="shared" si="0"/>
         <v>27.848101265822784</v>
       </c>
       <c r="E65" s="8" t="s">
@@ -4144,7 +4144,7 @@
         <v>1505</v>
       </c>
       <c r="D66" s="6">
-        <f>B66/C66*100</f>
+        <f t="shared" ref="D66:D129" si="1">B66/C66*100</f>
         <v>27.375415282392023</v>
       </c>
       <c r="E66" s="8" t="s">
@@ -4162,7 +4162,7 @@
         <v>1210</v>
       </c>
       <c r="D67" s="6">
-        <f>B67/C67*100</f>
+        <f t="shared" si="1"/>
         <v>27.355371900826448</v>
       </c>
       <c r="E67" s="8">
@@ -4180,7 +4180,7 @@
         <v>2215</v>
       </c>
       <c r="D68" s="6">
-        <f>B68/C68*100</f>
+        <f t="shared" si="1"/>
         <v>27.178329571106097</v>
       </c>
       <c r="E68" s="8" t="s">
@@ -4198,7 +4198,7 @@
         <v>3276</v>
       </c>
       <c r="D69" s="6">
-        <f>B69/C69*100</f>
+        <f t="shared" si="1"/>
         <v>26.831501831501832</v>
       </c>
       <c r="E69" s="8" t="s">
@@ -4216,7 +4216,7 @@
         <v>4068</v>
       </c>
       <c r="D70" s="6">
-        <f>B70/C70*100</f>
+        <f t="shared" si="1"/>
         <v>26.769911504424783</v>
       </c>
       <c r="E70" s="8" t="s">
@@ -4234,7 +4234,7 @@
         <v>1013</v>
       </c>
       <c r="D71" s="6">
-        <f>B71/C71*100</f>
+        <f t="shared" si="1"/>
         <v>26.258637709772952</v>
       </c>
       <c r="E71" s="8">
@@ -4252,7 +4252,7 @@
         <v>1980</v>
       </c>
       <c r="D72" s="6">
-        <f>B72/C72*100</f>
+        <f t="shared" si="1"/>
         <v>26.212121212121215</v>
       </c>
       <c r="E72" s="8" t="s">
@@ -4270,7 +4270,7 @@
         <v>1599</v>
       </c>
       <c r="D73" s="6">
-        <f>B73/C73*100</f>
+        <f t="shared" si="1"/>
         <v>26.203877423389621</v>
       </c>
       <c r="E73" s="8">
@@ -4288,7 +4288,7 @@
         <v>1599</v>
       </c>
       <c r="D74" s="6">
-        <f>B74/C74*100</f>
+        <f t="shared" si="1"/>
         <v>26.203877423389621</v>
       </c>
       <c r="E74" s="8">
@@ -4306,7 +4306,7 @@
         <v>2106</v>
       </c>
       <c r="D75" s="6">
-        <f>B75/C75*100</f>
+        <f t="shared" si="1"/>
         <v>26.163342830009494</v>
       </c>
       <c r="E75" s="8" t="s">
@@ -4324,7 +4324,7 @@
         <v>1748</v>
       </c>
       <c r="D76" s="6">
-        <f>B76/C76*100</f>
+        <f t="shared" si="1"/>
         <v>26.144164759725403</v>
       </c>
       <c r="E76" s="8" t="s">
@@ -4342,7 +4342,7 @@
         <v>1530</v>
       </c>
       <c r="D77" s="6">
-        <f>B77/C77*100</f>
+        <f t="shared" si="1"/>
         <v>25.947712418300657</v>
       </c>
       <c r="E77" s="8" t="s">
@@ -4360,7 +4360,7 @@
         <v>1719</v>
       </c>
       <c r="D78" s="6">
-        <f>B78/C78*100</f>
+        <f t="shared" si="1"/>
         <v>25.887143688190811</v>
       </c>
       <c r="E78" s="8">
@@ -4378,7 +4378,7 @@
         <v>1045</v>
       </c>
       <c r="D79" s="6">
-        <f>B79/C79*100</f>
+        <f t="shared" si="1"/>
         <v>25.837320574162682</v>
       </c>
       <c r="E79" s="8">
@@ -4396,7 +4396,7 @@
         <v>1976</v>
       </c>
       <c r="D80" s="6">
-        <f>B80/C80*100</f>
+        <f t="shared" si="1"/>
         <v>25.404858299595141</v>
       </c>
       <c r="E80" s="8">
@@ -4414,7 +4414,7 @@
         <v>1976</v>
       </c>
       <c r="D81" s="6">
-        <f>B81/C81*100</f>
+        <f t="shared" si="1"/>
         <v>25.404858299595141</v>
       </c>
       <c r="E81" s="8">
@@ -4432,7 +4432,7 @@
         <v>1421</v>
       </c>
       <c r="D82" s="6">
-        <f>B82/C82*100</f>
+        <f t="shared" si="1"/>
         <v>25.404644616467277</v>
       </c>
       <c r="E82" s="8">
@@ -4450,7 +4450,7 @@
         <v>1175</v>
       </c>
       <c r="D83" s="6">
-        <f>B83/C83*100</f>
+        <f t="shared" si="1"/>
         <v>25.361702127659573</v>
       </c>
       <c r="E83" s="8" t="s">
@@ -4468,7 +4468,7 @@
         <v>1842</v>
       </c>
       <c r="D84" s="6">
-        <f>B84/C84*100</f>
+        <f t="shared" si="1"/>
         <v>24.864277958740498</v>
       </c>
       <c r="E84" s="8">
@@ -4486,7 +4486,7 @@
         <v>4691</v>
       </c>
       <c r="D85" s="6">
-        <f>B85/C85*100</f>
+        <f t="shared" si="1"/>
         <v>24.813472607120016</v>
       </c>
       <c r="E85" s="8" t="s">
@@ -4504,7 +4504,7 @@
         <v>437647</v>
       </c>
       <c r="D86" s="6">
-        <f>B86/C86*100</f>
+        <f t="shared" si="1"/>
         <v>24.718551709482757</v>
       </c>
       <c r="E86" s="8">
@@ -4522,7 +4522,7 @@
         <v>3267</v>
       </c>
       <c r="D87" s="6">
-        <f>B87/C87*100</f>
+        <f t="shared" si="1"/>
         <v>24.701561065197428</v>
       </c>
       <c r="E87" s="8" t="s">
@@ -4540,7 +4540,7 @@
         <v>1804</v>
       </c>
       <c r="D88" s="6">
-        <f>B88/C88*100</f>
+        <f t="shared" si="1"/>
         <v>24.611973392461199</v>
       </c>
       <c r="E88" s="8" t="s">
@@ -4558,7 +4558,7 @@
         <v>1044</v>
       </c>
       <c r="D89" s="6">
-        <f>B89/C89*100</f>
+        <f t="shared" si="1"/>
         <v>24.521072796934863</v>
       </c>
       <c r="E89" s="8">
@@ -4576,7 +4576,7 @@
         <v>1478</v>
       </c>
       <c r="D90" s="6">
-        <f>B90/C90*100</f>
+        <f t="shared" si="1"/>
         <v>24.492557510148849</v>
       </c>
       <c r="E90" s="8">
@@ -4594,7 +4594,7 @@
         <v>574</v>
       </c>
       <c r="D91" s="6">
-        <f>B91/C91*100</f>
+        <f t="shared" si="1"/>
         <v>24.390243902439025</v>
       </c>
       <c r="E91" s="8" t="s">
@@ -4612,7 +4612,7 @@
         <v>1746</v>
       </c>
       <c r="D92" s="6">
-        <f>B92/C92*100</f>
+        <f t="shared" si="1"/>
         <v>24.284077892325314</v>
       </c>
       <c r="E92" s="8" t="s">
@@ -4630,7 +4630,7 @@
         <v>2195</v>
       </c>
       <c r="D93" s="6">
-        <f>B93/C93*100</f>
+        <f t="shared" si="1"/>
         <v>24.236902050113894</v>
       </c>
       <c r="E93" s="8">
@@ -4648,7 +4648,7 @@
         <v>1673</v>
       </c>
       <c r="D94" s="6">
-        <f>B94/C94*100</f>
+        <f t="shared" si="1"/>
         <v>24.208009563658102</v>
       </c>
       <c r="E94" s="8">
@@ -4666,7 +4666,7 @@
         <v>997</v>
       </c>
       <c r="D95" s="6">
-        <f>B95/C95*100</f>
+        <f t="shared" si="1"/>
         <v>24.172517552657975</v>
       </c>
       <c r="E95" s="8">
@@ -4684,7 +4684,7 @@
         <v>1322</v>
       </c>
       <c r="D96" s="6">
-        <f>B96/C96*100</f>
+        <f t="shared" si="1"/>
         <v>24.05446293494705</v>
       </c>
       <c r="E96" s="8">
@@ -4702,7 +4702,7 @@
         <v>1322</v>
       </c>
       <c r="D97" s="6">
-        <f>B97/C97*100</f>
+        <f t="shared" si="1"/>
         <v>24.05446293494705</v>
       </c>
       <c r="E97" s="8">
@@ -4720,7 +4720,7 @@
         <v>1862</v>
       </c>
       <c r="D98" s="6">
-        <f>B98/C98*100</f>
+        <f t="shared" si="1"/>
         <v>24.006444683136412</v>
       </c>
       <c r="E98" s="8" t="s">
@@ -4738,7 +4738,7 @@
         <v>1764</v>
       </c>
       <c r="D99" s="6">
-        <f>B99/C99*100</f>
+        <f t="shared" si="1"/>
         <v>23.979591836734691</v>
       </c>
       <c r="E99" s="8" t="s">
@@ -4756,7 +4756,7 @@
         <v>1684</v>
       </c>
       <c r="D100" s="6">
-        <f>B100/C100*100</f>
+        <f t="shared" si="1"/>
         <v>23.931116389548691</v>
       </c>
       <c r="E100" s="8" t="s">
@@ -4774,7 +4774,7 @@
         <v>861</v>
       </c>
       <c r="D101" s="6">
-        <f>B101/C101*100</f>
+        <f t="shared" si="1"/>
         <v>23.925667828106853</v>
       </c>
       <c r="E101" s="8">
@@ -4792,7 +4792,7 @@
         <v>861</v>
       </c>
       <c r="D102" s="6">
-        <f>B102/C102*100</f>
+        <f t="shared" si="1"/>
         <v>23.925667828106853</v>
       </c>
       <c r="E102" s="8">
@@ -4810,7 +4810,7 @@
         <v>2195</v>
       </c>
       <c r="D103" s="6">
-        <f>B103/C103*100</f>
+        <f t="shared" si="1"/>
         <v>23.917995444191344</v>
       </c>
       <c r="E103" s="8">
@@ -4828,7 +4828,7 @@
         <v>1938</v>
       </c>
       <c r="D104" s="6">
-        <f>B104/C104*100</f>
+        <f t="shared" si="1"/>
         <v>23.787409700722396</v>
       </c>
       <c r="E104" s="8" t="s">
@@ -4846,7 +4846,7 @@
         <v>1484</v>
       </c>
       <c r="D105" s="6">
-        <f>B105/C105*100</f>
+        <f t="shared" si="1"/>
         <v>23.71967654986523</v>
       </c>
       <c r="E105" s="8" t="s">
@@ -4864,7 +4864,7 @@
         <v>1051</v>
       </c>
       <c r="D106" s="6">
-        <f>B106/C106*100</f>
+        <f t="shared" si="1"/>
         <v>23.596574690770694</v>
       </c>
       <c r="E106" s="8" t="s">
@@ -4882,7 +4882,7 @@
         <v>1463</v>
       </c>
       <c r="D107" s="6">
-        <f>B107/C107*100</f>
+        <f t="shared" si="1"/>
         <v>23.513328776486674</v>
       </c>
       <c r="E107" s="8">
@@ -4900,7 +4900,7 @@
         <v>1806</v>
       </c>
       <c r="D108" s="6">
-        <f>B108/C108*100</f>
+        <f t="shared" si="1"/>
         <v>23.477297895902545</v>
       </c>
       <c r="E108" s="8">
@@ -4918,7 +4918,7 @@
         <v>1171</v>
       </c>
       <c r="D109" s="6">
-        <f>B109/C109*100</f>
+        <f t="shared" si="1"/>
         <v>23.39880444064902</v>
       </c>
       <c r="E109" s="8">
@@ -4936,7 +4936,7 @@
         <v>1361</v>
       </c>
       <c r="D110" s="6">
-        <f>B110/C110*100</f>
+        <f t="shared" si="1"/>
         <v>23.291697281410727</v>
       </c>
       <c r="E110" s="8">
@@ -4954,7 +4954,7 @@
         <v>1094</v>
       </c>
       <c r="D111" s="6">
-        <f>B111/C111*100</f>
+        <f t="shared" si="1"/>
         <v>23.217550274223033</v>
       </c>
       <c r="E111" s="8">
@@ -4972,7 +4972,7 @@
         <v>1722</v>
       </c>
       <c r="D112" s="6">
-        <f>B112/C112*100</f>
+        <f t="shared" si="1"/>
         <v>23.170731707317074</v>
       </c>
       <c r="E112" s="8">
@@ -4990,7 +4990,7 @@
         <v>1408</v>
       </c>
       <c r="D113" s="6">
-        <f>B113/C113*100</f>
+        <f t="shared" si="1"/>
         <v>23.15340909090909</v>
       </c>
       <c r="E113" s="8">
@@ -5008,7 +5008,7 @@
         <v>1408</v>
       </c>
       <c r="D114" s="6">
-        <f>B114/C114*100</f>
+        <f t="shared" si="1"/>
         <v>23.15340909090909</v>
       </c>
       <c r="E114" s="8">
@@ -5026,7 +5026,7 @@
         <v>1247</v>
       </c>
       <c r="D115" s="6">
-        <f>B115/C115*100</f>
+        <f t="shared" si="1"/>
         <v>22.93504410585405</v>
       </c>
       <c r="E115" s="8" t="s">
@@ -5044,7 +5044,7 @@
         <v>2021</v>
       </c>
       <c r="D116" s="6">
-        <f>B116/C116*100</f>
+        <f t="shared" si="1"/>
         <v>22.909450766947057</v>
       </c>
       <c r="E116" s="8" t="s">
@@ -5062,7 +5062,7 @@
         <v>1573</v>
       </c>
       <c r="D117" s="6">
-        <f>B117/C117*100</f>
+        <f t="shared" si="1"/>
         <v>22.886204704386522</v>
       </c>
       <c r="E117" s="8" t="s">
@@ -5080,7 +5080,7 @@
         <v>2454</v>
       </c>
       <c r="D118" s="6">
-        <f>B118/C118*100</f>
+        <f t="shared" si="1"/>
         <v>22.697636511817439</v>
       </c>
       <c r="E118" s="8" t="s">
@@ -5098,7 +5098,7 @@
         <v>1049</v>
       </c>
       <c r="D119" s="6">
-        <f>B119/C119*100</f>
+        <f t="shared" si="1"/>
         <v>22.592945662535747</v>
       </c>
       <c r="E119" s="8">
@@ -5116,7 +5116,7 @@
         <v>912</v>
       </c>
       <c r="D120" s="6">
-        <f>B120/C120*100</f>
+        <f t="shared" si="1"/>
         <v>22.587719298245617</v>
       </c>
       <c r="E120" s="8">
@@ -5134,7 +5134,7 @@
         <v>912</v>
       </c>
       <c r="D121" s="6">
-        <f>B121/C121*100</f>
+        <f t="shared" si="1"/>
         <v>22.587719298245617</v>
       </c>
       <c r="E121" s="8">
@@ -5152,7 +5152,7 @@
         <v>1619</v>
       </c>
       <c r="D122" s="6">
-        <f>B122/C122*100</f>
+        <f t="shared" si="1"/>
         <v>22.544780728844966</v>
       </c>
       <c r="E122" s="8">
@@ -5170,7 +5170,7 @@
         <v>1334</v>
       </c>
       <c r="D123" s="6">
-        <f>B123/C123*100</f>
+        <f t="shared" si="1"/>
         <v>22.488755622188904</v>
       </c>
       <c r="E123" s="8">
@@ -5188,7 +5188,7 @@
         <v>1965</v>
       </c>
       <c r="D124" s="6">
-        <f>B124/C124*100</f>
+        <f t="shared" si="1"/>
         <v>22.442748091603054</v>
       </c>
       <c r="E124" s="8" t="s">
@@ -5206,7 +5206,7 @@
         <v>1188</v>
       </c>
       <c r="D125" s="6">
-        <f>B125/C125*100</f>
+        <f t="shared" si="1"/>
         <v>22.306397306397308</v>
       </c>
       <c r="E125" s="8">
@@ -5224,7 +5224,7 @@
         <v>1762</v>
       </c>
       <c r="D126" s="6">
-        <f>B126/C126*100</f>
+        <f t="shared" si="1"/>
         <v>22.304199772985246</v>
       </c>
       <c r="E126" s="8">
@@ -5242,7 +5242,7 @@
         <v>4053</v>
       </c>
       <c r="D127" s="6">
-        <f>B127/C127*100</f>
+        <f t="shared" si="1"/>
         <v>21.983715766099184</v>
       </c>
       <c r="E127" s="8" t="s">
@@ -5260,7 +5260,7 @@
         <v>1611</v>
       </c>
       <c r="D128" s="6">
-        <f>B128/C128*100</f>
+        <f t="shared" si="1"/>
         <v>21.911855990068279</v>
       </c>
       <c r="E128" s="8">
@@ -5278,7 +5278,7 @@
         <v>1611</v>
       </c>
       <c r="D129" s="6">
-        <f>B129/C129*100</f>
+        <f t="shared" si="1"/>
         <v>21.911855990068279</v>
       </c>
       <c r="E129" s="8">
@@ -5296,7 +5296,7 @@
         <v>1303</v>
       </c>
       <c r="D130" s="6">
-        <f>B130/C130*100</f>
+        <f t="shared" ref="D130:D193" si="2">B130/C130*100</f>
         <v>21.872601688411358</v>
       </c>
       <c r="E130" s="8">
@@ -5314,7 +5314,7 @@
         <v>751</v>
       </c>
       <c r="D131" s="6">
-        <f>B131/C131*100</f>
+        <f t="shared" si="2"/>
         <v>21.837549933422103</v>
       </c>
       <c r="E131" s="8">
@@ -5332,7 +5332,7 @@
         <v>751</v>
       </c>
       <c r="D132" s="6">
-        <f>B132/C132*100</f>
+        <f t="shared" si="2"/>
         <v>21.837549933422103</v>
       </c>
       <c r="E132" s="8">
@@ -5350,7 +5350,7 @@
         <v>1429</v>
       </c>
       <c r="D133" s="6">
-        <f>B133/C133*100</f>
+        <f t="shared" si="2"/>
         <v>21.833449965010495</v>
       </c>
       <c r="E133" s="8">
@@ -5368,7 +5368,7 @@
         <v>2336</v>
       </c>
       <c r="D134" s="6">
-        <f>B134/C134*100</f>
+        <f t="shared" si="2"/>
         <v>21.789383561643834</v>
       </c>
       <c r="E134" s="8" t="s">
@@ -5386,7 +5386,7 @@
         <v>1905</v>
       </c>
       <c r="D135" s="6">
-        <f>B135/C135*100</f>
+        <f t="shared" si="2"/>
         <v>21.627296587926509</v>
       </c>
       <c r="E135" s="8" t="s">
@@ -5404,7 +5404,7 @@
         <v>1794</v>
       </c>
       <c r="D136" s="6">
-        <f>B136/C136*100</f>
+        <f t="shared" si="2"/>
         <v>21.57190635451505</v>
       </c>
       <c r="E136" s="8">
@@ -5422,7 +5422,7 @@
         <v>2242</v>
       </c>
       <c r="D137" s="6">
-        <f>B137/C137*100</f>
+        <f t="shared" si="2"/>
         <v>21.498661909009812</v>
       </c>
       <c r="E137" s="8">
@@ -5440,7 +5440,7 @@
         <v>1552</v>
       </c>
       <c r="D138" s="6">
-        <f>B138/C138*100</f>
+        <f t="shared" si="2"/>
         <v>21.391752577319586</v>
       </c>
       <c r="E138" s="8" t="s">
@@ -5458,7 +5458,7 @@
         <v>1132</v>
       </c>
       <c r="D139" s="6">
-        <f>B139/C139*100</f>
+        <f t="shared" si="2"/>
         <v>21.378091872791519</v>
       </c>
       <c r="E139" s="8">
@@ -5476,7 +5476,7 @@
         <v>5211</v>
       </c>
       <c r="D140" s="6">
-        <f>B140/C140*100</f>
+        <f t="shared" si="2"/>
         <v>21.301093839953943</v>
       </c>
       <c r="E140" s="8" t="s">
@@ -5494,7 +5494,7 @@
         <v>2137</v>
       </c>
       <c r="D141" s="6">
-        <f>B141/C141*100</f>
+        <f t="shared" si="2"/>
         <v>21.244735610669164</v>
       </c>
       <c r="E141" s="8">
@@ -5512,7 +5512,7 @@
         <v>2137</v>
       </c>
       <c r="D142" s="6">
-        <f>B142/C142*100</f>
+        <f t="shared" si="2"/>
         <v>21.244735610669164</v>
       </c>
       <c r="E142" s="8">
@@ -5530,7 +5530,7 @@
         <v>2218</v>
       </c>
       <c r="D143" s="6">
-        <f>B143/C143*100</f>
+        <f t="shared" si="2"/>
         <v>21.235347159603247</v>
       </c>
       <c r="E143" s="8" t="s">
@@ -5548,7 +5548,7 @@
         <v>1188</v>
       </c>
       <c r="D144" s="6">
-        <f>B144/C144*100</f>
+        <f t="shared" si="2"/>
         <v>21.043771043771045</v>
       </c>
       <c r="E144" s="8">
@@ -5566,7 +5566,7 @@
         <v>1188</v>
       </c>
       <c r="D145" s="6">
-        <f>B145/C145*100</f>
+        <f t="shared" si="2"/>
         <v>21.043771043771045</v>
       </c>
       <c r="E145" s="8">
@@ -5584,7 +5584,7 @@
         <v>1133</v>
       </c>
       <c r="D146" s="6">
-        <f>B146/C146*100</f>
+        <f t="shared" si="2"/>
         <v>21.006178287731686</v>
       </c>
       <c r="E146" s="8">
@@ -5602,7 +5602,7 @@
         <v>1133</v>
       </c>
       <c r="D147" s="6">
-        <f>B147/C147*100</f>
+        <f t="shared" si="2"/>
         <v>21.006178287731686</v>
       </c>
       <c r="E147" s="8">
@@ -5620,7 +5620,7 @@
         <v>2165</v>
       </c>
       <c r="D148" s="6">
-        <f>B148/C148*100</f>
+        <f t="shared" si="2"/>
         <v>20.969976905311778</v>
       </c>
       <c r="E148" s="8" t="s">
@@ -5638,7 +5638,7 @@
         <v>2323</v>
       </c>
       <c r="D149" s="6">
-        <f>B149/C149*100</f>
+        <f t="shared" si="2"/>
         <v>20.749031424881618</v>
       </c>
       <c r="E149" s="8">
@@ -5656,7 +5656,7 @@
         <v>3392</v>
       </c>
       <c r="D150" s="6">
-        <f>B150/C150*100</f>
+        <f t="shared" si="2"/>
         <v>20.725235849056602</v>
       </c>
       <c r="E150" s="8" t="s">
@@ -5674,7 +5674,7 @@
         <v>1455</v>
       </c>
       <c r="D151" s="6">
-        <f>B151/C151*100</f>
+        <f t="shared" si="2"/>
         <v>20.687285223367695</v>
       </c>
       <c r="E151" s="8">
@@ -5692,7 +5692,7 @@
         <v>1397</v>
       </c>
       <c r="D152" s="6">
-        <f>B152/C152*100</f>
+        <f t="shared" si="2"/>
         <v>20.544022906227628</v>
       </c>
       <c r="E152" s="8">
@@ -5710,7 +5710,7 @@
         <v>1397</v>
       </c>
       <c r="D153" s="6">
-        <f>B153/C153*100</f>
+        <f t="shared" si="2"/>
         <v>20.544022906227628</v>
       </c>
       <c r="E153" s="8">
@@ -5728,7 +5728,7 @@
         <v>7282</v>
       </c>
       <c r="D154" s="6">
-        <f>B154/C154*100</f>
+        <f t="shared" si="2"/>
         <v>20.543806646525681</v>
       </c>
       <c r="E154" s="8" t="s">
@@ -5746,7 +5746,7 @@
         <v>2120</v>
       </c>
       <c r="D155" s="6">
-        <f>B155/C155*100</f>
+        <f t="shared" si="2"/>
         <v>20.518867924528301</v>
       </c>
       <c r="E155" s="8" t="s">
@@ -5764,7 +5764,7 @@
         <v>1418</v>
       </c>
       <c r="D156" s="6">
-        <f>B156/C156*100</f>
+        <f t="shared" si="2"/>
         <v>20.451339915373765</v>
       </c>
       <c r="E156" s="8">
@@ -5782,7 +5782,7 @@
         <v>1418</v>
       </c>
       <c r="D157" s="6">
-        <f>B157/C157*100</f>
+        <f t="shared" si="2"/>
         <v>20.451339915373765</v>
       </c>
       <c r="E157" s="8">
@@ -5800,7 +5800,7 @@
         <v>1443</v>
       </c>
       <c r="D158" s="6">
-        <f>B158/C158*100</f>
+        <f t="shared" si="2"/>
         <v>20.443520443520445</v>
       </c>
       <c r="E158" s="8">
@@ -5818,7 +5818,7 @@
         <v>1603</v>
       </c>
       <c r="D159" s="6">
-        <f>B159/C159*100</f>
+        <f t="shared" si="2"/>
         <v>20.399251403618216</v>
       </c>
       <c r="E159" s="8">
@@ -5836,7 +5836,7 @@
         <v>1263</v>
       </c>
       <c r="D160" s="6">
-        <f>B160/C160*100</f>
+        <f t="shared" si="2"/>
         <v>20.348376880443389</v>
       </c>
       <c r="E160" s="8">
@@ -5854,7 +5854,7 @@
         <v>1263</v>
       </c>
       <c r="D161" s="6">
-        <f>B161/C161*100</f>
+        <f t="shared" si="2"/>
         <v>20.348376880443389</v>
       </c>
       <c r="E161" s="8">
@@ -5872,7 +5872,7 @@
         <v>1728</v>
       </c>
       <c r="D162" s="6">
-        <f>B162/C162*100</f>
+        <f t="shared" si="2"/>
         <v>20.138888888888889</v>
       </c>
       <c r="E162" s="8" t="s">
@@ -5890,7 +5890,7 @@
         <v>1130</v>
       </c>
       <c r="D163" s="6">
-        <f>B163/C163*100</f>
+        <f t="shared" si="2"/>
         <v>20.088495575221238</v>
       </c>
       <c r="E163" s="8">
@@ -5908,7 +5908,7 @@
         <v>1130</v>
       </c>
       <c r="D164" s="6">
-        <f>B164/C164*100</f>
+        <f t="shared" si="2"/>
         <v>20.088495575221238</v>
       </c>
       <c r="E164" s="8">
@@ -5926,7 +5926,7 @@
         <v>1316</v>
       </c>
       <c r="D165" s="6">
-        <f>B165/C165*100</f>
+        <f t="shared" si="2"/>
         <v>19.984802431610944</v>
       </c>
       <c r="E165" s="8">
@@ -5944,7 +5944,7 @@
         <v>1316</v>
       </c>
       <c r="D166" s="6">
-        <f>B166/C166*100</f>
+        <f t="shared" si="2"/>
         <v>19.984802431610944</v>
       </c>
       <c r="E166" s="8">
@@ -5962,7 +5962,7 @@
         <v>1310</v>
       </c>
       <c r="D167" s="6">
-        <f>B167/C167*100</f>
+        <f t="shared" si="2"/>
         <v>19.923664122137406</v>
       </c>
       <c r="E167" s="8">
@@ -5980,7 +5980,7 @@
         <v>1310</v>
       </c>
       <c r="D168" s="6">
-        <f>B168/C168*100</f>
+        <f t="shared" si="2"/>
         <v>19.923664122137406</v>
       </c>
       <c r="E168" s="8">
@@ -5998,7 +5998,7 @@
         <v>2120</v>
       </c>
       <c r="D169" s="6">
-        <f>B169/C169*100</f>
+        <f t="shared" si="2"/>
         <v>19.764150943396228</v>
       </c>
       <c r="E169" s="8">
@@ -6016,7 +6016,7 @@
         <v>1357</v>
       </c>
       <c r="D170" s="6">
-        <f>B170/C170*100</f>
+        <f t="shared" si="2"/>
         <v>19.602063375092115</v>
       </c>
       <c r="E170" s="8">
@@ -6034,7 +6034,7 @@
         <v>1592</v>
       </c>
       <c r="D171" s="6">
-        <f>B171/C171*100</f>
+        <f t="shared" si="2"/>
         <v>19.535175879396984</v>
       </c>
       <c r="E171" s="8" t="s">
@@ -6052,7 +6052,7 @@
         <v>1461</v>
       </c>
       <c r="D172" s="6">
-        <f>B172/C172*100</f>
+        <f t="shared" si="2"/>
         <v>19.507186858316221</v>
       </c>
       <c r="E172" s="8" t="s">
@@ -6070,7 +6070,7 @@
         <v>1669</v>
       </c>
       <c r="D173" s="6">
-        <f>B173/C173*100</f>
+        <f t="shared" si="2"/>
         <v>19.472738166566806</v>
       </c>
       <c r="E173" s="8" t="s">
@@ -6088,7 +6088,7 @@
         <v>2275</v>
       </c>
       <c r="D174" s="6">
-        <f>B174/C174*100</f>
+        <f t="shared" si="2"/>
         <v>19.384615384615383</v>
       </c>
       <c r="E174" s="8" t="s">
@@ -6106,7 +6106,7 @@
         <v>2164</v>
       </c>
       <c r="D175" s="6">
-        <f>B175/C175*100</f>
+        <f t="shared" si="2"/>
         <v>19.085027726432532</v>
       </c>
       <c r="E175" s="8" t="s">
@@ -6124,7 +6124,7 @@
         <v>1654</v>
       </c>
       <c r="D176" s="6">
-        <f>B176/C176*100</f>
+        <f t="shared" si="2"/>
         <v>19.044740024183795</v>
       </c>
       <c r="E176" s="8">
@@ -6142,7 +6142,7 @@
         <v>1151</v>
       </c>
       <c r="D177" s="6">
-        <f>B177/C177*100</f>
+        <f t="shared" si="2"/>
         <v>19.026933101650741</v>
       </c>
       <c r="E177" s="8">
@@ -6160,7 +6160,7 @@
         <v>936</v>
       </c>
       <c r="D178" s="6">
-        <f>B178/C178*100</f>
+        <f t="shared" si="2"/>
         <v>19.017094017094017</v>
       </c>
       <c r="E178" s="8">
@@ -6178,7 +6178,7 @@
         <v>3340</v>
       </c>
       <c r="D179" s="6">
-        <f>B179/C179*100</f>
+        <f t="shared" si="2"/>
         <v>19.011976047904191</v>
       </c>
       <c r="E179" s="8" t="s">
@@ -6196,7 +6196,7 @@
         <v>769</v>
       </c>
       <c r="D180" s="6">
-        <f>B180/C180*100</f>
+        <f t="shared" si="2"/>
         <v>18.985695708712612</v>
       </c>
       <c r="E180" s="8" t="s">
@@ -6214,7 +6214,7 @@
         <v>1196</v>
       </c>
       <c r="D181" s="6">
-        <f>B181/C181*100</f>
+        <f t="shared" si="2"/>
         <v>18.979933110367895</v>
       </c>
       <c r="E181" s="8">
@@ -6232,7 +6232,7 @@
         <v>2722</v>
       </c>
       <c r="D182" s="6">
-        <f>B182/C182*100</f>
+        <f t="shared" si="2"/>
         <v>18.88317413666422</v>
       </c>
       <c r="E182" s="8">
@@ -6250,7 +6250,7 @@
         <v>3206</v>
       </c>
       <c r="D183" s="6">
-        <f>B183/C183*100</f>
+        <f t="shared" si="2"/>
         <v>18.839675608234561</v>
       </c>
       <c r="E183" s="8" t="s">
@@ -6268,7 +6268,7 @@
         <v>1525</v>
       </c>
       <c r="D184" s="6">
-        <f>B184/C184*100</f>
+        <f t="shared" si="2"/>
         <v>18.622950819672131</v>
       </c>
       <c r="E184" s="8">
@@ -6286,7 +6286,7 @@
         <v>1525</v>
       </c>
       <c r="D185" s="6">
-        <f>B185/C185*100</f>
+        <f t="shared" si="2"/>
         <v>18.622950819672131</v>
       </c>
       <c r="E185" s="8">
@@ -6304,7 +6304,7 @@
         <v>1336</v>
       </c>
       <c r="D186" s="6">
-        <f>B186/C186*100</f>
+        <f t="shared" si="2"/>
         <v>18.488023952095809</v>
       </c>
       <c r="E186" s="8">
@@ -6322,7 +6322,7 @@
         <v>1711</v>
       </c>
       <c r="D187" s="6">
-        <f>B187/C187*100</f>
+        <f t="shared" si="2"/>
         <v>18.351841028638223</v>
       </c>
       <c r="E187" s="8">
@@ -6340,7 +6340,7 @@
         <v>1148</v>
       </c>
       <c r="D188" s="6">
-        <f>B188/C188*100</f>
+        <f t="shared" si="2"/>
         <v>18.292682926829269</v>
       </c>
       <c r="E188" s="8">
@@ -6358,7 +6358,7 @@
         <v>1148</v>
       </c>
       <c r="D189" s="6">
-        <f>B189/C189*100</f>
+        <f t="shared" si="2"/>
         <v>18.292682926829269</v>
       </c>
       <c r="E189" s="8">
@@ -6376,7 +6376,7 @@
         <v>1320</v>
       </c>
       <c r="D190" s="6">
-        <f>B190/C190*100</f>
+        <f t="shared" si="2"/>
         <v>18.257575757575758</v>
       </c>
       <c r="E190" s="8">
@@ -6394,7 +6394,7 @@
         <v>1995</v>
       </c>
       <c r="D191" s="6">
-        <f>B191/C191*100</f>
+        <f t="shared" si="2"/>
         <v>18.245614035087719</v>
       </c>
       <c r="E191" s="8">
@@ -6412,7 +6412,7 @@
         <v>1283</v>
       </c>
       <c r="D192" s="6">
-        <f>B192/C192*100</f>
+        <f t="shared" si="2"/>
         <v>18.23850350740452</v>
       </c>
       <c r="E192" s="8" t="s">
@@ -6430,7 +6430,7 @@
         <v>1027</v>
       </c>
       <c r="D193" s="6">
-        <f>B193/C193*100</f>
+        <f t="shared" si="2"/>
         <v>18.208373904576437</v>
       </c>
       <c r="E193" s="8">
@@ -6448,7 +6448,7 @@
         <v>1027</v>
       </c>
       <c r="D194" s="6">
-        <f>B194/C194*100</f>
+        <f t="shared" ref="D194:D257" si="3">B194/C194*100</f>
         <v>18.208373904576437</v>
       </c>
       <c r="E194" s="8">
@@ -6466,7 +6466,7 @@
         <v>1221</v>
       </c>
       <c r="D195" s="6">
-        <f>B195/C195*100</f>
+        <f t="shared" si="3"/>
         <v>18.181818181818183</v>
       </c>
       <c r="E195" s="8" t="s">
@@ -6484,7 +6484,7 @@
         <v>1694</v>
       </c>
       <c r="D196" s="6">
-        <f>B196/C196*100</f>
+        <f t="shared" si="3"/>
         <v>18.181818181818183</v>
       </c>
       <c r="E196" s="8">
@@ -6502,7 +6502,7 @@
         <v>1694</v>
       </c>
       <c r="D197" s="6">
-        <f>B197/C197*100</f>
+        <f t="shared" si="3"/>
         <v>18.181818181818183</v>
       </c>
       <c r="E197" s="8">
@@ -6520,7 +6520,7 @@
         <v>1411</v>
       </c>
       <c r="D198" s="6">
-        <f>B198/C198*100</f>
+        <f t="shared" si="3"/>
         <v>18.072289156626507</v>
       </c>
       <c r="E198" s="8" t="s">
@@ -6538,7 +6538,7 @@
         <v>2331</v>
       </c>
       <c r="D199" s="6">
-        <f>B199/C199*100</f>
+        <f t="shared" si="3"/>
         <v>17.846417846417847</v>
       </c>
       <c r="E199" s="8" t="s">
@@ -6556,7 +6556,7 @@
         <v>1272</v>
       </c>
       <c r="D200" s="6">
-        <f>B200/C200*100</f>
+        <f t="shared" si="3"/>
         <v>17.845911949685533</v>
       </c>
       <c r="E200" s="8">
@@ -6574,7 +6574,7 @@
         <v>1728</v>
       </c>
       <c r="D201" s="6">
-        <f>B201/C201*100</f>
+        <f t="shared" si="3"/>
         <v>17.824074074074073</v>
       </c>
       <c r="E201" s="8" t="s">
@@ -6592,7 +6592,7 @@
         <v>2919</v>
       </c>
       <c r="D202" s="6">
-        <f>B202/C202*100</f>
+        <f t="shared" si="3"/>
         <v>17.814319972593353</v>
       </c>
       <c r="E202" s="8" t="s">
@@ -6610,7 +6610,7 @@
         <v>1167</v>
       </c>
       <c r="D203" s="6">
-        <f>B203/C203*100</f>
+        <f t="shared" si="3"/>
         <v>17.737789203084834</v>
       </c>
       <c r="E203" s="8">
@@ -6628,7 +6628,7 @@
         <v>1167</v>
       </c>
       <c r="D204" s="6">
-        <f>B204/C204*100</f>
+        <f t="shared" si="3"/>
         <v>17.737789203084834</v>
       </c>
       <c r="E204" s="8">
@@ -6646,7 +6646,7 @@
         <v>654</v>
       </c>
       <c r="D205" s="6">
-        <f>B205/C205*100</f>
+        <f t="shared" si="3"/>
         <v>17.737003058103976</v>
       </c>
       <c r="E205" s="8">
@@ -6664,7 +6664,7 @@
         <v>1907</v>
       </c>
       <c r="D206" s="6">
-        <f>B206/C206*100</f>
+        <f t="shared" si="3"/>
         <v>17.671735710540116</v>
       </c>
       <c r="E206" s="8" t="s">
@@ -6682,7 +6682,7 @@
         <v>3313</v>
       </c>
       <c r="D207" s="6">
-        <f>B207/C207*100</f>
+        <f t="shared" si="3"/>
         <v>17.627527920313916</v>
       </c>
       <c r="E207" s="8" t="s">
@@ -6700,7 +6700,7 @@
         <v>2685</v>
       </c>
       <c r="D208" s="6">
-        <f>B208/C208*100</f>
+        <f t="shared" si="3"/>
         <v>17.616387337057731</v>
       </c>
       <c r="E208" s="8">
@@ -6718,7 +6718,7 @@
         <v>2864</v>
       </c>
       <c r="D209" s="6">
-        <f>B209/C209*100</f>
+        <f t="shared" si="3"/>
         <v>17.562849162011172</v>
       </c>
       <c r="E209" s="8">
@@ -6736,7 +6736,7 @@
         <v>1660</v>
       </c>
       <c r="D210" s="6">
-        <f>B210/C210*100</f>
+        <f t="shared" si="3"/>
         <v>17.46987951807229</v>
       </c>
       <c r="E210" s="8" t="s">
@@ -6754,7 +6754,7 @@
         <v>2003</v>
       </c>
       <c r="D211" s="6">
-        <f>B211/C211*100</f>
+        <f t="shared" si="3"/>
         <v>17.373939091362956</v>
       </c>
       <c r="E211" s="8">
@@ -6772,7 +6772,7 @@
         <v>7716</v>
       </c>
       <c r="D212" s="6">
-        <f>B212/C212*100</f>
+        <f t="shared" si="3"/>
         <v>16.796267496111973</v>
       </c>
       <c r="E212" s="8" t="s">
@@ -6790,7 +6790,7 @@
         <v>1501</v>
       </c>
       <c r="D213" s="6">
-        <f>B213/C213*100</f>
+        <f t="shared" si="3"/>
         <v>16.722185209860093</v>
       </c>
       <c r="E213" s="8" t="s">
@@ -6808,7 +6808,7 @@
         <v>1239</v>
       </c>
       <c r="D214" s="6">
-        <f>B214/C214*100</f>
+        <f t="shared" si="3"/>
         <v>16.707021791767556</v>
       </c>
       <c r="E214" s="8">
@@ -6826,7 +6826,7 @@
         <v>819</v>
       </c>
       <c r="D215" s="6">
-        <f>B215/C215*100</f>
+        <f t="shared" si="3"/>
         <v>16.605616605616603</v>
       </c>
       <c r="E215" s="8">
@@ -6844,7 +6844,7 @@
         <v>819</v>
       </c>
       <c r="D216" s="6">
-        <f>B216/C216*100</f>
+        <f t="shared" si="3"/>
         <v>16.605616605616603</v>
       </c>
       <c r="E216" s="8">
@@ -6862,7 +6862,7 @@
         <v>2041</v>
       </c>
       <c r="D217" s="6">
-        <f>B217/C217*100</f>
+        <f t="shared" si="3"/>
         <v>16.560509554140125</v>
       </c>
       <c r="E217" s="8" t="s">
@@ -6880,7 +6880,7 @@
         <v>1366</v>
       </c>
       <c r="D218" s="6">
-        <f>B218/C218*100</f>
+        <f t="shared" si="3"/>
         <v>16.544655929721817</v>
       </c>
       <c r="E218" s="8">
@@ -6898,7 +6898,7 @@
         <v>2366</v>
       </c>
       <c r="D219" s="6">
-        <f>B219/C219*100</f>
+        <f t="shared" si="3"/>
         <v>16.441251056635672</v>
       </c>
       <c r="E219" s="8" t="s">
@@ -6916,7 +6916,7 @@
         <v>958</v>
       </c>
       <c r="D220" s="6">
-        <f>B220/C220*100</f>
+        <f t="shared" si="3"/>
         <v>16.388308977035489</v>
       </c>
       <c r="E220" s="8" t="s">
@@ -6934,7 +6934,7 @@
         <v>1185</v>
       </c>
       <c r="D221" s="6">
-        <f>B221/C221*100</f>
+        <f t="shared" si="3"/>
         <v>16.371308016877638</v>
       </c>
       <c r="E221" s="8" t="s">
@@ -6952,7 +6952,7 @@
         <v>2184</v>
       </c>
       <c r="D222" s="6">
-        <f>B222/C222*100</f>
+        <f t="shared" si="3"/>
         <v>16.208791208791208</v>
       </c>
       <c r="E222" s="8">
@@ -6970,7 +6970,7 @@
         <v>2184</v>
       </c>
       <c r="D223" s="6">
-        <f>B223/C223*100</f>
+        <f t="shared" si="3"/>
         <v>16.208791208791208</v>
       </c>
       <c r="E223" s="8">
@@ -6988,7 +6988,7 @@
         <v>1088</v>
       </c>
       <c r="D224" s="6">
-        <f>B224/C224*100</f>
+        <f t="shared" si="3"/>
         <v>16.176470588235293</v>
       </c>
       <c r="E224" s="8">
@@ -7006,7 +7006,7 @@
         <v>2731</v>
       </c>
       <c r="D225" s="6">
-        <f>B225/C225*100</f>
+        <f t="shared" si="3"/>
         <v>16.111314536799707</v>
       </c>
       <c r="E225" s="8">
@@ -7024,7 +7024,7 @@
         <v>1649</v>
       </c>
       <c r="D226" s="6">
-        <f>B226/C226*100</f>
+        <f t="shared" si="3"/>
         <v>16.070345664038811</v>
       </c>
       <c r="E226" s="8" t="s">
@@ -7042,7 +7042,7 @@
         <v>1558</v>
       </c>
       <c r="D227" s="6">
-        <f>B227/C227*100</f>
+        <f t="shared" si="3"/>
         <v>16.046213093709884</v>
       </c>
       <c r="E227" s="8" t="s">
@@ -7060,7 +7060,7 @@
         <v>1136</v>
       </c>
       <c r="D228" s="6">
-        <f>B228/C228*100</f>
+        <f t="shared" si="3"/>
         <v>16.02112676056338</v>
       </c>
       <c r="E228" s="8" t="s">
@@ -7078,7 +7078,7 @@
         <v>1706</v>
       </c>
       <c r="D229" s="6">
-        <f>B229/C229*100</f>
+        <f t="shared" si="3"/>
         <v>15.885111371629543</v>
       </c>
       <c r="E229" s="8">
@@ -7096,7 +7096,7 @@
         <v>1518</v>
       </c>
       <c r="D230" s="6">
-        <f>B230/C230*100</f>
+        <f t="shared" si="3"/>
         <v>15.876152832674572</v>
       </c>
       <c r="E230" s="8" t="s">
@@ -7114,7 +7114,7 @@
         <v>1896</v>
       </c>
       <c r="D231" s="6">
-        <f>B231/C231*100</f>
+        <f t="shared" si="3"/>
         <v>15.875527426160337</v>
       </c>
       <c r="E231" s="8">
@@ -7132,7 +7132,7 @@
         <v>1405</v>
       </c>
       <c r="D232" s="6">
-        <f>B232/C232*100</f>
+        <f t="shared" si="3"/>
         <v>15.871886120996443</v>
       </c>
       <c r="E232" s="8">
@@ -7150,7 +7150,7 @@
         <v>2405</v>
       </c>
       <c r="D233" s="6">
-        <f>B233/C233*100</f>
+        <f t="shared" si="3"/>
         <v>15.592515592515593</v>
       </c>
       <c r="E233" s="8">
@@ -7168,7 +7168,7 @@
         <v>1645</v>
       </c>
       <c r="D234" s="6">
-        <f>B234/C234*100</f>
+        <f t="shared" si="3"/>
         <v>15.562310030395137</v>
       </c>
       <c r="E234" s="8" t="s">
@@ -7186,7 +7186,7 @@
         <v>1105</v>
       </c>
       <c r="D235" s="6">
-        <f>B235/C235*100</f>
+        <f t="shared" si="3"/>
         <v>15.475113122171946</v>
       </c>
       <c r="E235" s="8">
@@ -7204,7 +7204,7 @@
         <v>1555</v>
       </c>
       <c r="D236" s="6">
-        <f>B236/C236*100</f>
+        <f t="shared" si="3"/>
         <v>15.434083601286176</v>
       </c>
       <c r="E236" s="8">
@@ -7222,7 +7222,7 @@
         <v>1860</v>
       </c>
       <c r="D237" s="6">
-        <f>B237/C237*100</f>
+        <f t="shared" si="3"/>
         <v>15.161290322580644</v>
       </c>
       <c r="E237" s="8" t="s">
@@ -7240,7 +7240,7 @@
         <v>1417</v>
       </c>
       <c r="D238" s="6">
-        <f>B238/C238*100</f>
+        <f t="shared" si="3"/>
         <v>14.961185603387438</v>
       </c>
       <c r="E238" s="8" t="s">
@@ -7258,7 +7258,7 @@
         <v>1479</v>
       </c>
       <c r="D239" s="6">
-        <f>B239/C239*100</f>
+        <f t="shared" si="3"/>
         <v>14.942528735632186</v>
       </c>
       <c r="E239" s="8" t="s">
@@ -7276,7 +7276,7 @@
         <v>1426</v>
       </c>
       <c r="D240" s="6">
-        <f>B240/C240*100</f>
+        <f t="shared" si="3"/>
         <v>14.866760168302944</v>
       </c>
       <c r="E240" s="8" t="s">
@@ -7294,7 +7294,7 @@
         <v>1456</v>
       </c>
       <c r="D241" s="6">
-        <f>B241/C241*100</f>
+        <f t="shared" si="3"/>
         <v>14.560439560439562</v>
       </c>
       <c r="E241" s="8">
@@ -7312,7 +7312,7 @@
         <v>1456</v>
       </c>
       <c r="D242" s="6">
-        <f>B242/C242*100</f>
+        <f t="shared" si="3"/>
         <v>14.560439560439562</v>
       </c>
       <c r="E242" s="8">
@@ -7330,7 +7330,7 @@
         <v>2151</v>
       </c>
       <c r="D243" s="6">
-        <f>B243/C243*100</f>
+        <f t="shared" si="3"/>
         <v>14.458391445839144</v>
       </c>
       <c r="E243" s="8">
@@ -7348,7 +7348,7 @@
         <v>1090</v>
       </c>
       <c r="D244" s="6">
-        <f>B244/C244*100</f>
+        <f t="shared" si="3"/>
         <v>14.403669724770642</v>
       </c>
       <c r="E244" s="8">
@@ -7366,7 +7366,7 @@
         <v>2323</v>
       </c>
       <c r="D245" s="6">
-        <f>B245/C245*100</f>
+        <f t="shared" si="3"/>
         <v>14.248816185966422</v>
       </c>
       <c r="E245" s="8" t="s">
@@ -7384,7 +7384,7 @@
         <v>1510</v>
       </c>
       <c r="D246" s="6">
-        <f>B246/C246*100</f>
+        <f t="shared" si="3"/>
         <v>14.172185430463577</v>
       </c>
       <c r="E246" s="8">
@@ -7402,7 +7402,7 @@
         <v>2005</v>
       </c>
       <c r="D247" s="6">
-        <f>B247/C247*100</f>
+        <f t="shared" si="3"/>
         <v>14.164588528678305</v>
       </c>
       <c r="E247" s="8">
@@ -7420,7 +7420,7 @@
         <v>1520</v>
       </c>
       <c r="D248" s="6">
-        <f>B248/C248*100</f>
+        <f t="shared" si="3"/>
         <v>13.881578947368419</v>
       </c>
       <c r="E248" s="8" t="s">
@@ -7438,7 +7438,7 @@
         <v>2077</v>
       </c>
       <c r="D249" s="6">
-        <f>B249/C249*100</f>
+        <f t="shared" si="3"/>
         <v>13.818006740491093</v>
       </c>
       <c r="E249" s="8">
@@ -7456,7 +7456,7 @@
         <v>1786</v>
       </c>
       <c r="D250" s="6">
-        <f>B250/C250*100</f>
+        <f t="shared" si="3"/>
         <v>13.213885778275476</v>
       </c>
       <c r="E250" s="8">
@@ -7474,7 +7474,7 @@
         <v>1634</v>
       </c>
       <c r="D251" s="6">
-        <f>B251/C251*100</f>
+        <f t="shared" si="3"/>
         <v>12.668298653610771</v>
       </c>
       <c r="E251" s="8">
@@ -7492,7 +7492,7 @@
         <v>1222</v>
       </c>
       <c r="D252" s="6">
-        <f>B252/C252*100</f>
+        <f t="shared" si="3"/>
         <v>10.72013093289689</v>
       </c>
       <c r="E252" s="8">
@@ -7510,7 +7510,7 @@
         <v>1468</v>
       </c>
       <c r="D253" s="6">
-        <f>B253/C253*100</f>
+        <f t="shared" si="3"/>
         <v>10.354223433242508</v>
       </c>
       <c r="E253" s="8">
@@ -7528,7 +7528,7 @@
         <v>1032</v>
       </c>
       <c r="D254" s="6">
-        <f>B254/C254*100</f>
+        <f t="shared" si="3"/>
         <v>8.3333333333333321</v>
       </c>
       <c r="E254" s="8" t="s">
@@ -7546,7 +7546,7 @@
         <v>465</v>
       </c>
       <c r="D255" s="6">
-        <f>B255/C255*100</f>
+        <f t="shared" si="3"/>
         <v>7.956989247311828</v>
       </c>
       <c r="E255" s="8" t="s">
@@ -7564,7 +7564,7 @@
         <v>794</v>
       </c>
       <c r="D256" s="6">
-        <f>B256/C256*100</f>
+        <f t="shared" si="3"/>
         <v>5.7934508816120909</v>
       </c>
       <c r="E256" s="8">
@@ -7582,7 +7582,7 @@
         <v>1</v>
       </c>
       <c r="D257" s="6">
-        <f>B257/C257*100</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="E257" s="8" t="s">
@@ -7590,11 +7590,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E257" xr:uid="{99A89D46-FAA1-6C4D-8644-778B6623030C}">
-    <sortState ref="A2:E257">
-      <sortCondition ref="D2:D257"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:E257" xr:uid="{99A89D46-FAA1-6C4D-8644-778B6623030C}"/>
   <sortState ref="A2:E260">
     <sortCondition descending="1" ref="D1"/>
   </sortState>

</xml_diff>